<commit_message>
s and marriage use contains
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johntran/Desktop/workspace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johntran/GitClone/laodongkynghi-autofill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F7CAA2-8D97-AE42-BAD1-FB2BCDDF6C30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1F507C-3B86-9446-B2E4-D62B5D3945BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4380" yWindow="1920" windowWidth="28040" windowHeight="17440" xr2:uid="{9158847D-CD1C-4841-B494-79F2FD5561A2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>FullName</t>
   </si>
@@ -226,18 +226,6 @@
     <t>Chú thích</t>
   </si>
   <si>
-    <t>1: Nam, 2: Nữ</t>
-  </si>
-  <si>
-    <t>1: Độc thân, 2: Kết hôn, 3: Ly hôn</t>
-  </si>
-  <si>
-    <t>1: Chưa TN, 2: TN</t>
-  </si>
-  <si>
-    <t>1:  CQ, 2: Không CQ</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -303,6 +291,211 @@
   </si>
   <si>
     <t>Hoàn Kiếm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Điền chính xác </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nam</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hoặc </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nữ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nhập chính xác: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Độc thân</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hoặc </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kết hôn</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hoặc </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ly hôn</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Chưa tốt nghiệp, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Đã tốt nghiệp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:  CQ, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Không CQ</t>
+    </r>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Độc thân</t>
   </si>
 </sst>
 </file>
@@ -735,7 +928,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,11 +975,11 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
+      <c r="B4" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -816,10 +1009,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -838,10 +1031,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -849,10 +1042,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -924,10 +1117,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -949,7 +1142,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>